<commit_message>
Excepciones cuando los campos no se habilitan
</commit_message>
<xml_diff>
--- a/src/test/java/helpers/Assignee_Data.xlsx
+++ b/src/test/java/helpers/Assignee_Data.xlsx
@@ -3,12 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB3BAAD4-C637-4EB6-9D83-D5EACCD2B116}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42907BF4-2F70-469E-B8F5-7A5676A067CC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="NoState" sheetId="1" r:id="rId1"/>
+    <sheet name="State" sheetId="2" r:id="rId2"/>
+    <sheet name="Dependents" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="27">
   <si>
     <t>Scenario</t>
   </si>
@@ -80,6 +82,27 @@
   </si>
   <si>
     <t>CP Plus PPT</t>
+  </si>
+  <si>
+    <t>Home_State</t>
+  </si>
+  <si>
+    <t>Host_State</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>Alberta</t>
+  </si>
+  <si>
+    <t>Alabama</t>
+  </si>
+  <si>
+    <t>Dependents</t>
   </si>
 </sst>
 </file>
@@ -132,10 +155,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,8 +443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,4 +599,201 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7271BCF2-BE7D-432D-8482-D32AB698340F}">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2">
+        <v>87000</v>
+      </c>
+      <c r="E2" s="3">
+        <v>43101</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3">
+        <v>58900</v>
+      </c>
+      <c r="E3" s="3">
+        <v>43101</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CC72575-7534-4C5B-8510-5DF2231608F2}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>45000</v>
+      </c>
+      <c r="E2" s="2">
+        <v>43101</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>78000</v>
+      </c>
+      <c r="E3" s="2">
+        <v>43101</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="4">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>